<commit_message>
Se agregó archivo de cámara para eyetracker nuevo
</commit_message>
<xml_diff>
--- a/Transformaciones.xlsx
+++ b/Transformaciones.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9a9cf9957cfd094d/Escritorio/Chaya^JPaula - Proyecto de Graduacion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="79" documentId="11_AD4D2F04E46CFB4ACB3E208F5551C290683EDF1B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{91946436-644B-4EB1-9102-CDF9758DE2F8}"/>
+  <xr:revisionPtr revIDLastSave="109" documentId="11_AD4D2F04E46CFB4ACB3E208F5551C290683EDF1B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E4EC12E2-58A8-49A3-8B15-C5A3AE093AB4}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="1950" yWindow="1950" windowWidth="15375" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -30,13 +30,13 @@
     <t>Pixel</t>
   </si>
   <si>
-    <t>valor normalizado</t>
-  </si>
-  <si>
     <t>Transformaciones en eje X</t>
   </si>
   <si>
     <t>Transformaciones en eje Y</t>
+  </si>
+  <si>
+    <t>Valor en mm</t>
   </si>
 </sst>
 </file>
@@ -103,10 +103,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -159,8 +159,13 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="es-AR"/>
-              <a:t>Normalizacion</a:t>
+              <a:t>Relación</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="es-AR" baseline="0"/>
+              <a:t> píxel - milímetro en pantalla</a:t>
+            </a:r>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -195,7 +200,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.13404265987219433"/>
+          <c:y val="0.20556947427026165"/>
+          <c:w val="0.80369348584718847"/>
+          <c:h val="0.70020281555714636"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -243,8 +258,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-3.6297462817147859E-2"/>
-                  <c:y val="-4.2315908428113176E-2"/>
+                  <c:x val="0.23107774138852114"/>
+                  <c:y val="6.2838845144356961E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -287,7 +302,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>700</c:v>
+                  <c:v>768</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -299,10 +314,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>-110</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -358,8 +373,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-3.7213035870516185E-2"/>
-                  <c:y val="-3.7686278798483526E-2"/>
+                  <c:x val="-5.2366153345876014E-2"/>
+                  <c:y val="-2.2622222222222221E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -402,7 +417,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1300</c:v>
+                  <c:v>1360</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -414,10 +429,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>-200</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -603,7 +618,7 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="es-AR" baseline="0"/>
-                  <a:t> Normalizado</a:t>
+                  <a:t> en milímetros</a:t>
                 </a:r>
                 <a:endParaRPr lang="es-AR"/>
               </a:p>
@@ -687,37 +702,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-AR"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -1323,15 +1307,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:colOff>514349</xdr:colOff>
+      <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1625,7 +1609,7 @@
   <dimension ref="B1:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="B1" sqref="B1:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1634,33 +1618,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
-        <v>2</v>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
       </c>
-      <c r="C1" s="2"/>
+      <c r="C1" s="4"/>
     </row>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>1</v>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>0</v>
       </c>
-      <c r="C3" s="3">
-        <v>0</v>
+      <c r="C3" s="2">
+        <v>-200</v>
       </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="3">
-        <v>1300</v>
+      <c r="B4" s="2">
+        <v>1360</v>
       </c>
-      <c r="C4" s="3">
-        <v>1</v>
+      <c r="C4" s="2">
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
@@ -1668,37 +1652,37 @@
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
-        <v>3</v>
+      <c r="B6" s="4" t="s">
+        <v>2</v>
       </c>
-      <c r="C6" s="2"/>
+      <c r="C6" s="4"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>1</v>
+      <c r="C7" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>0</v>
       </c>
-      <c r="C8" s="3">
-        <v>0</v>
+      <c r="C8" s="2">
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="3">
-        <v>700</v>
+      <c r="B9" s="2">
+        <v>768</v>
       </c>
-      <c r="C9" s="3">
-        <v>1</v>
+      <c r="C9" s="2">
+        <v>-110</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="N16" s="4"/>
+      <c r="N16" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>